<commit_message>
Add manual re-fetch button for Google Fit steps
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -633,36 +633,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Subject</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Hours</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Minutes</t>
         </is>
@@ -709,6 +709,7 @@
           <t>dfg</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
         <v>50</v>
       </c>
@@ -729,6 +730,7 @@
           <t>df</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>300</v>
       </c>
@@ -749,6 +751,7 @@
           <t>dfg</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
         <v>300</v>
       </c>
@@ -769,6 +772,7 @@
           <t>d</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>100</v>
       </c>
@@ -789,6 +793,7 @@
           <t>erf</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
         <v>40</v>
       </c>
@@ -809,6 +814,7 @@
           <t>DCN</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
         <v>1</v>
       </c>
@@ -829,6 +835,7 @@
           <t>DCN</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
         <v>1</v>
       </c>
@@ -849,6 +856,7 @@
           <t>PHP</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
         <v>53</v>
       </c>
@@ -869,6 +877,7 @@
           <t>dcn</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
         <v>1</v>
       </c>
@@ -889,6 +898,7 @@
           <t>dcn</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
         <v>43</v>
       </c>
@@ -909,6 +919,7 @@
           <t>dcn</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
         <v>43</v>
       </c>
@@ -929,6 +940,7 @@
           <t>php</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
         <v>150</v>
       </c>
@@ -949,6 +961,7 @@
           <t>Mini Project</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
         <v>50</v>
       </c>
@@ -969,6 +982,7 @@
           <t>php</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
         <v>55</v>
       </c>
@@ -989,6 +1003,7 @@
           <t>phpe</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
         <v>20</v>
       </c>
@@ -1009,6 +1024,7 @@
           <t>lan</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
         <v>60</v>
       </c>
@@ -1029,6 +1045,7 @@
           <t>php</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
         <v>15</v>
       </c>
@@ -1049,6 +1066,7 @@
           <t>phpe</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
         <v>10</v>
       </c>
@@ -1069,6 +1087,7 @@
           <t>lan</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
         <v>50</v>
       </c>
@@ -1089,6 +1108,7 @@
           <t>lan</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
         <v>60</v>
       </c>
@@ -1109,7 +1129,50 @@
           <t>Mini Project</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Mini Project</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>php</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1272,8 +1335,6 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1296,8 +1357,6 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1325,7 +1384,6 @@
           <t>2025-12-31</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1392,7 +1450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1701,6 +1759,40 @@
         </is>
       </c>
       <c r="C18" t="inlineStr">
+        <is>
+          <t>gym</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>gym</t>
         </is>

</xml_diff>

<commit_message>
Task email notification added
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -852,7 +852,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -914,33 +914,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>manishmanoj006@gmail.com</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2026-02-08</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added productivity score, smart suggestions, and priority-based email reminder scheduler
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,20 +15,27 @@
     <sheet name="Tasks" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -43,12 +49,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -61,14 +82,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -437,7 +463,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -501,7 +527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,22 +536,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>subject</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>minutes</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>date</t>
         </is>
@@ -542,15 +568,11 @@
           <t>php</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2026-02-08 00:00:00</t>
-        </is>
+      <c r="C2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>46061</v>
       </c>
     </row>
     <row r="3">
@@ -564,15 +586,65 @@
           <t>mini pro</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2026-02-08 00:00:00</t>
-        </is>
+      <c r="C3" t="n">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>46061</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>php</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>46068</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>php</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>46069</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mini pro</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>46069</v>
       </c>
     </row>
   </sheetData>
@@ -586,7 +658,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,17 +667,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>habit</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>date</t>
         </is>
@@ -676,6 +748,108 @@
       <c r="C5" t="inlineStr">
         <is>
           <t>2026-02-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>gym</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2026-02-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2026-02-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2026-02-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>gym</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
         </is>
       </c>
     </row>
@@ -699,7 +873,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>habit</t>
         </is>
@@ -750,7 +924,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -806,47 +980,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>attendance</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>manishmanoj006@gmail.com</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -861,29 +994,29 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Created_Date</t>
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>attendance</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>monthlygoal</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>minattendance</t>
         </is>
       </c>
     </row>
@@ -893,9 +1026,81 @@
           <t>manishmanoj006@gmail.com</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>manish</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>45</v>
+      </c>
+      <c r="E2" t="n">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Created_Date</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Last_Reminded</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>drive3</t>
+          <t>nxt</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -910,7 +1115,44 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2026-02-16 07:41:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>manishmanoj006@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2026-02-16 07:57:01</t>
         </is>
       </c>
     </row>

</xml_diff>